<commit_message>
Outputs added for 1 layer 100 epoch without attention
</commit_message>
<xml_diff>
--- a/project_files/ConvGRU_layer_1_no_Attention.xlsx
+++ b/project_files/ConvGRU_layer_1_no_Attention.xlsx
@@ -415,16 +415,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>16.57498516007301</v>
+        <v>17.95399530092467</v>
       </c>
       <c r="C2">
-        <v>8.578495979309082</v>
+        <v>10.27326774597168</v>
       </c>
       <c r="D2">
-        <v>5.67</v>
+        <v>6.62</v>
       </c>
       <c r="E2">
-        <v>0.9123337135841926</v>
+        <v>0.897160927841782</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -432,16 +432,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>14.75447506018963</v>
+        <v>14.76794118325206</v>
       </c>
       <c r="C3">
-        <v>10.06263256072998</v>
+        <v>11.66104507446289</v>
       </c>
       <c r="D3">
-        <v>6.54</v>
+        <v>7.37</v>
       </c>
       <c r="E3">
-        <v>0.9785016831013115</v>
+        <v>0.9784198060558088</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -449,16 +449,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>2.873528809001592</v>
+        <v>2.726909101693961</v>
       </c>
       <c r="C4">
-        <v>2.179253816604614</v>
+        <v>2.046104192733765</v>
       </c>
       <c r="D4">
-        <v>1.42</v>
+        <v>1.33</v>
       </c>
       <c r="E4">
-        <v>0.9463636546713555</v>
+        <v>0.9505789800433458</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -466,16 +466,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>2.873528809001592</v>
+        <v>2.726811438621243</v>
       </c>
       <c r="C5">
-        <v>2.179253816604614</v>
+        <v>2.045972108840942</v>
       </c>
       <c r="D5">
-        <v>1.42</v>
+        <v>1.33</v>
       </c>
       <c r="E5">
-        <v>0.9463636546713555</v>
+        <v>0.9505824899917691</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -483,16 +483,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>13.20091050215619</v>
+        <v>12.5821658639182</v>
       </c>
       <c r="C6">
-        <v>7.450199604034424</v>
+        <v>7.802381992340088</v>
       </c>
       <c r="D6">
-        <v>6.75</v>
+        <v>7.08</v>
       </c>
       <c r="E6">
-        <v>0.8431352710230516</v>
+        <v>0.8575052819786672</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -500,16 +500,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>8.175817176969558</v>
+        <v>8.572147475475944</v>
       </c>
       <c r="C7">
-        <v>5.125075817108154</v>
+        <v>6.120565414428711</v>
       </c>
       <c r="D7">
-        <v>2.82</v>
+        <v>3.33</v>
       </c>
       <c r="E7">
-        <v>0.9365425252540091</v>
+        <v>0.9302316218366755</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -517,16 +517,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>12.22148644130332</v>
+        <v>9.165929267585415</v>
       </c>
       <c r="C8">
-        <v>8.128766059875488</v>
+        <v>6.710178375244141</v>
       </c>
       <c r="D8">
-        <v>5.8</v>
+        <v>5.1</v>
       </c>
       <c r="E8">
-        <v>0.8812517899476372</v>
+        <v>0.9331685600847157</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -534,16 +534,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>16.70883814682508</v>
+        <v>13.90801812407679</v>
       </c>
       <c r="C9">
-        <v>11.28981399536133</v>
+        <v>9.660391807556152</v>
       </c>
       <c r="D9">
-        <v>10.63</v>
+        <v>9.970000000000001</v>
       </c>
       <c r="E9">
-        <v>0.7850883168208872</v>
+        <v>0.8511368282721031</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -551,16 +551,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>71.83945452578618</v>
+        <v>60.14815083465264</v>
       </c>
       <c r="C10">
-        <v>44.83363342285156</v>
+        <v>33.17148971557617</v>
       </c>
       <c r="D10">
-        <v>39.02</v>
+        <v>28.94</v>
       </c>
       <c r="E10">
-        <v>-1.209063983146727</v>
+        <v>-0.5487347116377804</v>
       </c>
     </row>
   </sheetData>

</xml_diff>